<commit_message>
Na added to main.m
</commit_message>
<xml_diff>
--- a/etwas.xlsx
+++ b/etwas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minahassanaghaei/Desktop/GitHub/Sturgeon-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amir/Documents/MATLAB/projects/personal/sturgeon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226F229F-9C0E-154D-B066-5FE6C459A83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3797C3-49DD-EA40-AE3A-39B336099CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="500" windowWidth="14260" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Columbia Hatchery, 2016</t>
+  </si>
+  <si>
+    <t>Na</t>
   </si>
 </sst>
 </file>
@@ -443,9 +446,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -483,9 +486,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -518,9 +521,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,9 +573,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -729,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -748,7 +785,7 @@
     <col min="11" max="11" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -779,8 +816,11 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -811,8 +851,11 @@
       <c r="J2" s="7">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
@@ -843,8 +886,11 @@
       <c r="J3" s="13">
         <v>41.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K3" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -875,8 +921,11 @@
       <c r="J4" s="14">
         <v>3.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K4" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -907,8 +956,11 @@
       <c r="J5" s="13">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K5" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -939,8 +991,11 @@
       <c r="J6" s="14">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K6" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -971,8 +1026,11 @@
       <c r="J7" s="13">
         <v>47.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K7" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1003,8 +1061,11 @@
       <c r="J8" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K8" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1035,8 +1096,11 @@
       <c r="J9" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K9" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1067,8 +1131,11 @@
       <c r="J10" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K10" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -1099,8 +1166,11 @@
       <c r="J11" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K11" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
@@ -1131,8 +1201,11 @@
       <c r="J12" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K12" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>30</v>
       </c>
@@ -1163,8 +1236,11 @@
       <c r="J13">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K13" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
@@ -1195,8 +1271,11 @@
       <c r="J14">
         <v>3.53</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K14" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>30</v>
       </c>
@@ -1226,6 +1305,9 @@
       </c>
       <c r="J15">
         <v>3.1</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
etwas changed with NA
</commit_message>
<xml_diff>
--- a/etwas.xlsx
+++ b/etwas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amir/Documents/MATLAB/projects/personal/sturgeon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minahassanaghaei/Desktop/GitHub/Sturgeon-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3797C3-49DD-EA40-AE3A-39B336099CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B99DA09-46C3-904D-A678-FC6146BA0FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="500" windowWidth="14260" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
   <si>
     <r>
       <rPr>
@@ -288,10 +288,16 @@
     <t>Webb, 2006</t>
   </si>
   <si>
-    <t>Columbia Hatchery, 2016</t>
-  </si>
-  <si>
     <t>Na</t>
+  </si>
+  <si>
+    <t>Columbia Hatchery, A, 2016</t>
+  </si>
+  <si>
+    <t>Columbia Hatchery, B, 2016</t>
+  </si>
+  <si>
+    <t>Columbia Hatchery, C, 2016</t>
   </si>
 </sst>
 </file>
@@ -446,9 +452,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -486,9 +492,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,26 +527,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -573,26 +562,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -769,7 +741,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -817,7 +789,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1205,9 +1177,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>25</v>
@@ -1236,13 +1208,13 @@
       <c r="J13">
         <v>3.18</v>
       </c>
-      <c r="K13" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="K13" s="13">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>25</v>
@@ -1271,13 +1243,13 @@
       <c r="J14">
         <v>3.53</v>
       </c>
-      <c r="K14" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="K14" s="13">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>25</v>
@@ -1306,8 +1278,8 @@
       <c r="J15">
         <v>3.1</v>
       </c>
-      <c r="K15" s="13" t="s">
-        <v>26</v>
+      <c r="K15" s="13">
+        <v>1010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major changes applied to etwas
</commit_message>
<xml_diff>
--- a/etwas.xlsx
+++ b/etwas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minahassanaghaei/Desktop/GitHub/Sturgeon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amir/Documents/MATLAB/projects/personal/sturgeon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441DFA66-8228-4F43-AFA3-C433BB3F5D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E48B420-7D62-6244-8945-A97B9F1F0153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="2020" windowWidth="14260" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -310,6 +310,18 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>MacDonald</t>
+  </si>
+  <si>
+    <t>Webb</t>
+  </si>
+  <si>
+    <t>Columbia Hatchery</t>
   </si>
 </sst>
 </file>
@@ -464,9 +476,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -504,9 +516,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,9 +551,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,9 +603,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,26 +796,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C13" sqref="C13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="24.796875" customWidth="1"/>
-    <col min="2" max="3" width="9.3984375" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" customWidth="1"/>
-    <col min="5" max="7" width="9.3984375" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" customWidth="1"/>
-    <col min="9" max="9" width="9.3984375" customWidth="1"/>
-    <col min="10" max="10" width="10.3984375" customWidth="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" customWidth="1"/>
+    <col min="6" max="8" width="9.3984375" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" customWidth="1"/>
+    <col min="10" max="10" width="9.3984375" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -777,37 +825,40 @@
         <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -815,75 +866,81 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>78.8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>0.122</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>0.25600000000000001</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>0.57499999999999996</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>2.76</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="10">
+      <c r="E3" s="10">
         <v>68</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G3" s="11">
         <v>1.0900000000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>0.69599999999999995</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="13">
         <v>26.9</v>
       </c>
-      <c r="I3" s="14">
+      <c r="J3" s="14">
         <v>1.37</v>
       </c>
-      <c r="J3" s="14">
+      <c r="K3" s="14">
         <v>0.34</v>
       </c>
-      <c r="K3" s="13">
+      <c r="L3" s="13">
         <v>41.5</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -891,75 +948,81 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="13">
+      <c r="E4" s="13">
         <v>78.400000000000006</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4" s="12">
         <v>0.125</v>
       </c>
-      <c r="H4" s="12">
+      <c r="I4" s="12">
         <v>0.376</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="14">
         <v>1.42</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="14">
+      <c r="L4" s="14">
         <v>3.09</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="M4" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="11" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="13">
+      <c r="E5" s="13">
         <v>66.2</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="13">
         <v>0.3</v>
       </c>
-      <c r="G5" s="12">
+      <c r="H5" s="12">
         <v>0.54500000000000004</v>
       </c>
-      <c r="H5" s="14">
+      <c r="I5" s="14">
         <v>7.21</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="14">
         <v>1.24</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="13">
         <v>18.100000000000001</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -967,75 +1030,81 @@
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="13">
+      <c r="E6" s="13">
         <v>78.400000000000006</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="12">
         <v>0.10199999999999999</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I6" s="12">
         <v>0.24399999999999999</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="14">
         <v>0.18</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="14">
+      <c r="L6" s="14">
         <v>3.33</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="13">
+      <c r="E7" s="13">
         <v>63.2</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="14">
+      <c r="G7" s="14">
         <v>0.34</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H7" s="12">
         <v>0.33800000000000002</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="13">
         <v>24.7</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="14">
         <v>0.16</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="13">
+      <c r="L7" s="13">
         <v>47.4</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1043,11 +1112,11 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
@@ -1060,35 +1129,38 @@
       <c r="H8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="14">
         <v>0.27</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="K8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="13">
+      <c r="E9" s="13">
         <v>68.8</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="F9" s="9" t="s">
         <v>21</v>
       </c>
@@ -1098,35 +1170,38 @@
       <c r="H9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="14">
         <v>0.83</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="K9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="13">
+      <c r="E10" s="13">
         <v>45.9</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="9" t="s">
         <v>21</v>
       </c>
@@ -1136,20 +1211,23 @@
       <c r="H10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="14">
         <v>0.44</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="K10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -1157,14 +1235,14 @@
         <v>25</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>50</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" s="15" t="s">
         <v>26</v>
       </c>
@@ -1174,20 +1252,23 @@
       <c r="H11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11">
         <v>0.17</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="K11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
@@ -1195,14 +1276,14 @@
         <v>27</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>50</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="F12" s="15" t="s">
         <v>26</v>
       </c>
@@ -1212,20 +1293,23 @@
       <c r="H12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J12" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="K12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>31</v>
       </c>
@@ -1233,37 +1317,40 @@
         <v>25</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>80</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.16800000000000001</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>2.3E-3</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>9.4E-2</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.36</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>6.2700000000000006E-2</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>3.18</v>
       </c>
-      <c r="L13" s="13">
+      <c r="M13" s="13">
         <v>1450</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
@@ -1271,37 +1358,40 @@
         <v>25</v>
       </c>
       <c r="C14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>80</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.217</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.30099999999999999</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1.9E-3</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>3.53</v>
       </c>
-      <c r="L14" s="13">
+      <c r="M14" s="13">
         <v>1400</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
@@ -1309,33 +1399,36 @@
         <v>25</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>80</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.20899999999999999</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.05</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.22</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.1</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>1.9E-3</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>3.1</v>
       </c>
-      <c r="L15" s="13">
+      <c r="M15" s="13">
         <v>1010</v>
       </c>
     </row>

</xml_diff>